<commit_message>
Update with new keymapping
-Removed Spotify from button 4
-Added macro to hold spacebar
-Added macro to rapidly click M1
</commit_message>
<xml_diff>
--- a/Key Mapping/Razer Key Map Visualized.xlsx
+++ b/Key Mapping/Razer Key Map Visualized.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wally\Desktop\Razer Macro Batch Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0886DD-B045-4173-8041-357712001196}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99BBEE7-EE83-48FB-A417-C8E763164401}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{B99DB57F-DE64-469A-A205-C55C7CDB3DC4}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Key</t>
   </si>
@@ -98,10 +98,6 @@
   </si>
   <si>
     <t>Discord MUTE MIC</t>
-  </si>
-  <si>
-    <t>4
-Open Spotify</t>
   </si>
   <si>
     <t>1
@@ -172,6 +168,14 @@
   </si>
   <si>
     <t>Thumb Large</t>
+  </si>
+  <si>
+    <t>3
+Rapidly Click M1</t>
+  </si>
+  <si>
+    <t>4
+Hold Spacebar Down</t>
   </si>
 </sst>
 </file>
@@ -362,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -394,12 +398,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -417,18 +415,27 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,7 +974,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,42 +986,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="A1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
     </row>
     <row r="2" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
       </c>
-      <c r="C2" s="4">
-        <v>3</v>
+      <c r="C2" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="E2" s="4">
         <v>5</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
     </row>
     <row r="3" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -1023,105 +1030,105 @@
       <c r="B3" s="4">
         <v>7</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="25">
         <v>8</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="25">
         <v>9</v>
       </c>
       <c r="E3" s="4">
         <v>10</v>
       </c>
-      <c r="F3" s="12"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
+        <v>38</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
     </row>
     <row r="4" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="22"/>
+      <c r="G4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="16"/>
-      <c r="I4" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
     </row>
     <row r="5" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="C5" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>34</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
+        <v>29</v>
+      </c>
+      <c r="F5" s="22"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>